<commit_message>
cập nhật lại phân chia công việc
</commit_message>
<xml_diff>
--- a/Phân chia công việc - QLBH.xlsx
+++ b/Phân chia công việc - QLBH.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\QLBHSTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>STT</t>
   </si>
@@ -95,31 +95,19 @@
     <t>Xây dựng module tìm kiếm hàng theo các tiêu chí nào đó</t>
   </si>
   <si>
-    <t>Xây dựng module thống kê hàng hóa trong kho, lưu lượng nhập bán</t>
-  </si>
-  <si>
     <t>Xây dựng module quản lý khách hàng</t>
   </si>
   <si>
     <t>Xây dựng module quản lý nhân viên</t>
   </si>
   <si>
-    <t>Xây dựng module hướng dẫn sử dụng phần mềm (menu Help, F1) chi tiết đến từng chức năng</t>
-  </si>
-  <si>
-    <t>Xây dựng tài liệu hướng dẫn cài đặt, vận hành</t>
-  </si>
-  <si>
     <t>1.10</t>
   </si>
   <si>
-    <t>1.11</t>
-  </si>
-  <si>
-    <t>1.12</t>
-  </si>
-  <si>
     <t>Lào - Campuchia</t>
+  </si>
+  <si>
+    <t>Xây dựng module thống kê hàng hóa trong kho</t>
   </si>
 </sst>
 </file>
@@ -196,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,6 +222,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,21 +515,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -563,7 +561,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="2">
         <v>1.1000000000000001</v>
@@ -579,7 +577,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="3:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="2">
         <v>1.2</v>
@@ -593,7 +591,7 @@
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="2">
         <v>1.3</v>
@@ -607,7 +605,7 @@
       </c>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="2">
         <v>1.4</v>
@@ -621,7 +619,7 @@
       </c>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
       <c r="D11" s="2">
         <v>1.5</v>
@@ -635,13 +633,13 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="2">
         <v>1.6</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4" t="s">
@@ -649,13 +647,13 @@
       </c>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
       <c r="D13" s="9">
         <v>1.7</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="12" t="s">
@@ -663,13 +661,13 @@
       </c>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="8"/>
       <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="12" t="s">
@@ -677,61 +675,49 @@
       </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="3:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C15" s="7"/>
       <c r="D15" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C16" s="7"/>
       <c r="D16" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="12" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="D17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="7"/>
+    <row r="17" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>